<commit_message>
added to stats excel
</commit_message>
<xml_diff>
--- a/dnaSimulator/files/minion_idt/handling singletons stats.xlsx
+++ b/dnaSimulator/files/minion_idt/handling singletons stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\yoav\technion\spring 2022\project\git\DNASimulator\dnaSimulator\files\minion_idt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohadsmac/PycharmProjects/DNASimulator/dnaSimulator/files/minion_idt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C46E03F-A041-42F2-8EAB-36D7BAA9C534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1EF090-AEE9-464E-9653-154EF6C3DAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{04ABBE7A-D2AF-478C-B65A-3909A7CD5CCB}"/>
+    <workbookView xWindow="1360" yWindow="1120" windowWidth="25220" windowHeight="15840" activeTab="3" xr2:uid="{04ABBE7A-D2AF-478C-B65A-3909A7CD5CCB}"/>
   </bookViews>
   <sheets>
     <sheet name="3000 strands" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="33">
   <si>
     <t>3000 strands each od length 150 with x2.0 more errors</t>
   </si>
@@ -106,12 +105,6 @@
     <t>9000 strands each od length 150 with x2.0 more errors</t>
   </si>
   <si>
-    <t>uniun</t>
-  </si>
-  <si>
-    <t>singletons</t>
-  </si>
-  <si>
     <t>regular</t>
   </si>
   <si>
@@ -126,12 +119,30 @@
   <si>
     <t>avg time in minutes</t>
   </si>
+  <si>
+    <t>with uniun handling</t>
+  </si>
+  <si>
+    <t>with singleton handling</t>
+  </si>
+  <si>
+    <t>with union handling</t>
+  </si>
+  <si>
+    <t>Average Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strand length </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +189,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -214,13 +247,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +284,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1803400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BC62BC7-DB8D-7141-81B3-5BFBE3EFE3ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1803400" y="2311400"/>
+          <a:ext cx="3213100" cy="2717800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,27 +634,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39871FE5-5D1A-4A19-B079-9D65DCD244F8}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -569,15 +666,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -591,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -605,7 +702,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -619,7 +716,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -633,7 +730,7 @@
         <v>0.86070000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -643,7 +740,7 @@
         <v>4.6289999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -653,7 +750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -663,19 +760,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
         <v>6</v>
@@ -687,15 +784,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -709,7 +806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -723,7 +820,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -737,7 +834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -751,7 +848,7 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -761,7 +858,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -771,7 +868,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -781,7 +878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
         <v>6</v>
@@ -793,15 +890,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
@@ -815,7 +912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -829,7 +926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
@@ -843,7 +940,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>5</v>
       </c>
@@ -857,7 +954,7 @@
         <v>0.86770000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
@@ -867,7 +964,7 @@
         <v>1.617</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -877,7 +974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
@@ -887,7 +984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="3" t="s">
         <v>6</v>
@@ -899,15 +996,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
@@ -921,7 +1018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -935,7 +1032,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>4</v>
       </c>
@@ -949,7 +1046,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>5</v>
       </c>
@@ -963,7 +1060,7 @@
         <v>0.87729999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>11</v>
       </c>
@@ -973,7 +1070,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -983,7 +1080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -993,7 +1090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="3" t="s">
         <v>6</v>
@@ -1005,15 +1102,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>3</v>
       </c>
@@ -1041,7 +1138,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>4</v>
       </c>
@@ -1055,7 +1152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>5</v>
       </c>
@@ -1069,7 +1166,7 @@
         <v>0.87370000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1176,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>13</v>
       </c>
@@ -1099,7 +1196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="3" t="s">
         <v>6</v>
@@ -1111,15 +1208,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>2</v>
       </c>
@@ -1133,7 +1230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>3</v>
       </c>
@@ -1147,7 +1244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1258,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>5</v>
       </c>
@@ -1175,7 +1272,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>11</v>
       </c>
@@ -1185,7 +1282,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
@@ -1195,7 +1292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>13</v>
       </c>
@@ -1205,7 +1302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="3" t="s">
         <v>6</v>
@@ -1217,15 +1314,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>2</v>
       </c>
@@ -1239,7 +1336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>3</v>
       </c>
@@ -1253,7 +1350,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>4</v>
       </c>
@@ -1267,7 +1364,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>5</v>
       </c>
@@ -1281,7 +1378,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>11</v>
       </c>
@@ -1291,7 +1388,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>12</v>
       </c>
@@ -1301,7 +1398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>13</v>
       </c>
@@ -1311,7 +1408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="3" t="s">
         <v>6</v>
@@ -1323,15 +1420,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-    </row>
-    <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1470,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>5</v>
       </c>
@@ -1387,7 +1484,7 @@
         <v>0.86929999999999996</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>11</v>
       </c>
@@ -1397,7 +1494,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -1407,7 +1504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>13</v>
       </c>
@@ -1417,7 +1514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="3" t="s">
         <v>6</v>
@@ -1429,15 +1526,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>3</v>
       </c>
@@ -1465,7 +1562,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>4</v>
       </c>
@@ -1479,7 +1576,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>5</v>
       </c>
@@ -1493,7 +1590,7 @@
         <v>0.86570000000000003</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>11</v>
       </c>
@@ -1503,7 +1600,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>12</v>
       </c>
@@ -1513,7 +1610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>13</v>
       </c>
@@ -1546,27 +1643,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701BD6C-32EA-4AA3-875D-CB5E4D4D1FF9}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -1578,15 +1675,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1600,7 +1697,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1711,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1725,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1642,7 +1739,7 @@
         <v>0.86980000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1652,7 +1749,7 @@
         <v>1.7190000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1662,7 +1759,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1672,19 +1769,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
         <v>6</v>
@@ -1696,15 +1793,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1718,7 +1815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -1732,7 +1829,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1746,7 +1843,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -1760,7 +1857,7 @@
         <v>0.87150000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1867,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1780,7 +1877,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -1790,7 +1887,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="5" t="s">
         <v>6</v>
@@ -1802,15 +1899,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
@@ -1824,7 +1921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -1838,7 +1935,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +1949,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>5</v>
       </c>
@@ -1866,7 +1963,7 @@
         <v>0.86819999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
@@ -1876,7 +1973,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -1886,7 +1983,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
@@ -1896,7 +1993,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
         <v>6</v>
@@ -1908,15 +2005,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
@@ -1930,7 +2027,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -1944,7 +2041,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>4</v>
       </c>
@@ -1958,7 +2055,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>5</v>
       </c>
@@ -1972,7 +2069,7 @@
         <v>0.88149999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>11</v>
       </c>
@@ -1982,7 +2079,7 @@
         <v>1.645</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -1992,7 +2089,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -2002,7 +2099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="5" t="s">
         <v>6</v>
@@ -2014,15 +2111,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>2</v>
       </c>
@@ -2036,7 +2133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>3</v>
       </c>
@@ -2050,7 +2147,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>4</v>
       </c>
@@ -2064,7 +2161,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>5</v>
       </c>
@@ -2078,7 +2175,7 @@
         <v>0.86029999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>11</v>
       </c>
@@ -2088,7 +2185,7 @@
         <v>1.7450000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
@@ -2098,7 +2195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>13</v>
       </c>
@@ -2108,7 +2205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="5" t="s">
         <v>6</v>
@@ -2120,15 +2217,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>2</v>
       </c>
@@ -2142,7 +2239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>3</v>
       </c>
@@ -2156,7 +2253,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +2267,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>5</v>
       </c>
@@ -2184,7 +2281,7 @@
         <v>0.82769999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>11</v>
       </c>
@@ -2194,7 +2291,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
@@ -2204,7 +2301,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>13</v>
       </c>
@@ -2214,7 +2311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="5" t="s">
         <v>6</v>
@@ -2226,15 +2323,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>2</v>
       </c>
@@ -2248,7 +2345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>3</v>
       </c>
@@ -2262,7 +2359,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>4</v>
       </c>
@@ -2276,7 +2373,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>5</v>
       </c>
@@ -2290,7 +2387,7 @@
         <v>0.87770000000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>11</v>
       </c>
@@ -2300,7 +2397,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>12</v>
       </c>
@@ -2310,7 +2407,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>13</v>
       </c>
@@ -2320,7 +2417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="5" t="s">
         <v>6</v>
@@ -2332,15 +2429,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-    </row>
-    <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>2</v>
       </c>
@@ -2354,7 +2451,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>3</v>
       </c>
@@ -2368,7 +2465,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>4</v>
       </c>
@@ -2382,7 +2479,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>5</v>
       </c>
@@ -2396,7 +2493,7 @@
         <v>0.87780000000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>11</v>
       </c>
@@ -2406,7 +2503,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -2416,7 +2513,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>13</v>
       </c>
@@ -2426,7 +2523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="5" t="s">
         <v>6</v>
@@ -2438,15 +2535,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>2</v>
       </c>
@@ -2460,7 +2557,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2571,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>4</v>
       </c>
@@ -2488,7 +2585,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>5</v>
       </c>
@@ -2502,7 +2599,7 @@
         <v>0.87729999999999997</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>11</v>
       </c>
@@ -2512,7 +2609,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>12</v>
       </c>
@@ -2522,7 +2619,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>13</v>
       </c>
@@ -2553,27 +2650,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB74513-71E4-40FA-9163-D8432EC9D6C5}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -2585,15 +2682,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2704,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2621,7 +2718,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -2635,7 +2732,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -2649,7 +2746,7 @@
         <v>0.86919999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -2659,7 +2756,7 @@
         <v>1.7949999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2669,7 +2766,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -2679,19 +2776,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
         <v>6</v>
@@ -2703,15 +2800,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -2725,7 +2822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -2739,7 +2836,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -2753,7 +2850,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -2767,7 +2864,7 @@
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
@@ -2777,7 +2874,7 @@
         <v>1.7450000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2787,7 +2884,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -2797,7 +2894,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="5" t="s">
         <v>6</v>
@@ -2809,15 +2906,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>2</v>
       </c>
@@ -2831,7 +2928,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -2845,7 +2942,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
@@ -2859,7 +2956,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2873,7 +2970,7 @@
         <v>0.86060000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>11</v>
       </c>
@@ -2883,7 +2980,7 @@
         <v>1.6970000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -2893,7 +2990,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
@@ -2903,7 +3000,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
         <v>6</v>
@@ -2915,15 +3012,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
@@ -2937,7 +3034,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -2951,7 +3048,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>4</v>
       </c>
@@ -2965,7 +3062,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>5</v>
       </c>
@@ -2979,7 +3076,7 @@
         <v>0.85929999999999995</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +3086,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -2999,7 +3096,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -3009,271 +3106,271 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
     </row>
-    <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-    </row>
-    <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
     </row>
-    <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3298,43 +3395,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9EF424-B2C7-491A-9398-919056002DE1}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="2">
         <v>0.75649999999999995</v>
@@ -3345,10 +3461,22 @@
       <c r="D3" s="2">
         <v>2.9578000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>22</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.76</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.73499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="2">
         <v>5.6000000000000001E-2</v>
@@ -3359,10 +3487,22 @@
       <c r="D4" s="2">
         <v>0.17050000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>23</v>
+      <c r="E4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.76</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.76</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="2">
         <v>5.7365000000000004</v>
@@ -3373,12 +3513,90 @@
       <c r="D5" s="2">
         <v>62.139000000000003</v>
       </c>
+      <c r="E5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.88</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.87</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.86499999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>